<commit_message>
Chose priors and implemented rejection algorithm to vary all
</commit_message>
<xml_diff>
--- a/documentation/priors.xlsx
+++ b/documentation/priors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nora Schmit\Documents\Model development\hbvmodel\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD29A2D-A23F-41C6-93E1-6008F30D1E0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B55CA-A68C-48E6-9570-7140F43ADEF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t>Parameter name</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Relative infectiousness of HBeAg-positives compared to HBeAg-negatives for horizontal transmission</t>
   </si>
   <si>
-    <t>Log-normal truncated at 1. 95% of mass below 15.</t>
-  </si>
-  <si>
     <t>alpha needs to be higher than 1 because eAg-positives are more infectious</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t xml:space="preserve">Annual progression rate from Immune tolerant to Immune reactive stage. This is the average progression rate at every age if eag_prog_function_intercept = 0, or the rate in 0-year olds otherwise. </t>
   </si>
   <si>
-    <t>around 0.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">pr_ir_ic </t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Annual progression rate from Immune reactive to HBeAg-negative chronic hepatitis B (HBeAg loss)</t>
   </si>
   <si>
-    <t>around 0.08 (very unlikely after that)</t>
-  </si>
-  <si>
     <t>pr_ir_cc_female</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
     <t>Annual progression rate from Compensatd cirrhosis to Decompensated cirrhosis (rate of decompensation)</t>
   </si>
   <si>
-    <t>around 0.15</t>
-  </si>
-  <si>
     <t>cancer_prog_coefficient_female</t>
   </si>
   <si>
@@ -247,21 +235,12 @@
     <t>Annual rate of additional mortality from Compensated cirrhosis</t>
   </si>
   <si>
-    <t>Beta with most mass around 0.026</t>
-  </si>
-  <si>
-    <t>Reference for centre is D'Amico 2006 (this was looking only at compensated without decompensation). Upper limit is from Shevanthi Gambia</t>
-  </si>
-  <si>
     <t xml:space="preserve">mu_dcc </t>
   </si>
   <si>
     <t>Annual rate of additional mortality from Deompensated cirrhosis</t>
   </si>
   <si>
-    <t>Beta with most mass around 0.5</t>
-  </si>
-  <si>
     <t>References for centre are Child Pugh score, D'Amico 2006 and Shevanthi Gambia</t>
   </si>
   <si>
@@ -280,12 +259,6 @@
     <t>Reference is Shevanthi's Gambia value and Hsu 2003, which was the value reported in males, so divided by 2 and 5 here to get the center in females</t>
   </si>
   <si>
-    <t>References are Boglione and Chu 2009</t>
-  </si>
-  <si>
-    <t>Log normal truncated at 1 and centered around 2-5</t>
-  </si>
-  <si>
     <t>Shevanthi expert opinion, REVEAL Chen and Yang 2011, Jing Sun 2017</t>
   </si>
   <si>
@@ -298,60 +271,18 @@
     <t>Coefficient of quadratic shift function for age-specific progression rates to HCC in women, represents the age-specific rate in inactive carriers. This describes the rate of increase in the progression rate with age. If 0, the progression rate to HCC from all carrier compartments does not change with age.</t>
   </si>
   <si>
-    <t>Truncated log normal</t>
-  </si>
-  <si>
     <t>hccr_it</t>
   </si>
   <si>
     <t>hccr_enchb</t>
   </si>
   <si>
-    <t>hccr_ir</t>
-  </si>
-  <si>
     <t>REVEAL viral load</t>
   </si>
   <si>
-    <t>Truncated log normal centered around 5</t>
-  </si>
-  <si>
-    <t>0 or 0.000125</t>
-  </si>
-  <si>
-    <t>Range based on Gambian studies CIs</t>
-  </si>
-  <si>
-    <t>Mimic Shevanthi's Gambia value for pr_it_ir: Beta(5.063, 45.57)</t>
-  </si>
-  <si>
     <t>Mimic Shevanthi's Gambia value: Beta(0.154,30.69)</t>
   </si>
   <si>
-    <t>Gamma centered vaguely around 0.015</t>
-  </si>
-  <si>
-    <t>Gamma with most mass around 0.006-0.015</t>
-  </si>
-  <si>
-    <t>Mimic Shevanthi's Gambia value: Beta(2.848, 70.18)</t>
-  </si>
-  <si>
-    <t>Gamma with most mass around 0.04</t>
-  </si>
-  <si>
-    <t>UNIFORM or gamma centered vaguely around 0.00022</t>
-  </si>
-  <si>
-    <t>Gamma vaguely centered around 0.08 or less</t>
-  </si>
-  <si>
-    <t>Beta strongly centered at 0.95</t>
-  </si>
-  <si>
-    <t>Gamma centered around 0.1 or slightly less</t>
-  </si>
-  <si>
     <t>Reference is Raffetti, coefficient value was chosen to empirically match their IC rate adjusted for a male cofactor of 2-5, as the mean rate in 30+ year olds.</t>
   </si>
   <si>
@@ -373,9 +304,6 @@
     <t>Multiplier on progression rate to HCC from Compensated cirrhosis stage compared to from Inactive carrier</t>
   </si>
   <si>
-    <t>Ref for center is Hui 2002, also Mittal for lower, Thiele for upper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Normal(0, 0.005)? </t>
   </si>
   <si>
@@ -409,23 +337,71 @@
     <t>Shevanthi's expert opinion</t>
   </si>
   <si>
-    <t>Beta(2,20) which has a mean of 0.09</t>
-  </si>
-  <si>
-    <t>Beta(14,2) which has a mean of 0.87</t>
-  </si>
-  <si>
-    <t>Gamma(2, 0.003) - centered at 0.006</t>
-  </si>
-  <si>
     <t>Reference for lower limit is Lin 2007 divided by 5 (male cofactor). Reference for upper limit is Shevanthi</t>
+  </si>
+  <si>
+    <t>Gamma(1.49, 97.58) - centered at 0.005</t>
+  </si>
+  <si>
+    <t>Beta(1.5,13.5) - mean of 0.1</t>
+  </si>
+  <si>
+    <t>Beta(10.49,1.3) - mean of 0.89</t>
+  </si>
+  <si>
+    <t>References are Boglione and Chu 2009 and Shevanthi</t>
+  </si>
+  <si>
+    <t>Gamma(3.12,141.30) - mode of 0.015</t>
+  </si>
+  <si>
+    <t>Gamma(2.3,123.8) - centered at 0.0105</t>
+  </si>
+  <si>
+    <t>Shevanthi's Gambia value, minimum chosen for biological plausibility (lifetime)</t>
+  </si>
+  <si>
+    <t>Gamma(3.63,26.27) - center at 0.1</t>
+  </si>
+  <si>
+    <t>Gamma(17.94,423.61) - center at 0.04</t>
+  </si>
+  <si>
+    <t>Shevanthi's Gambia value but with higher upper limit (D'Amico 2006)</t>
+  </si>
+  <si>
+    <t>Ref for center is Hui 2002, Thiele for range, also Mittal for lower</t>
+  </si>
+  <si>
+    <t>Gamma(8.09, 101.33) - center at 0.07</t>
+  </si>
+  <si>
+    <t>Reference for centre is D'Amico 2006 (this was looking only at compensated without decompensation but probably includes background mortality). Ref for upper limit is Lin 2005</t>
+  </si>
+  <si>
+    <t>Gamma(4.25, 124.91) - center at 0.026</t>
+  </si>
+  <si>
+    <t>Gamma(1.49, 0.98) - center at 0.5</t>
+  </si>
+  <si>
+    <t>Range vaguely based on Gambian studies CIs (min = 0.77). Center based on immunogenicity studies e.g. WHO position paper.</t>
+  </si>
+  <si>
+    <t>Beta(7.07, 0.37) - center at 0.95</t>
+  </si>
+  <si>
+    <t>Normal(3.5,4) truncated at 1 - center between 2 and 5</t>
+  </si>
+  <si>
+    <t>Normal(6,3) truncated at 1 - center at 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +545,13 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF010101"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -915,7 +898,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -924,6 +907,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1281,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1342,7 +1326,7 @@
         <v>0.7</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1401,22 +1385,25 @@
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
       <c r="C6">
         <v>0.6</v>
@@ -1425,27 +1412,27 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7">
         <v>0.05</v>
       </c>
-      <c r="E7" t="s">
-        <v>129</v>
+      <c r="E7" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1454,44 +1441,44 @@
         <v>0.3</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
       </c>
       <c r="C8">
         <v>0.89</v>
       </c>
-      <c r="E8" t="s">
-        <v>130</v>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F8">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
       </c>
       <c r="C9">
         <v>0.65</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>0.25</v>
@@ -1500,21 +1487,21 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
       </c>
       <c r="C10">
         <v>0.46</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F10">
         <v>0.1</v>
@@ -1523,38 +1510,38 @@
         <v>0.9</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
       </c>
       <c r="C11">
         <v>0.1</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <v>0.3</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>0.8</v>
@@ -1569,21 +1556,21 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="F13" s="2">
         <v>-0.01</v>
@@ -1592,38 +1579,38 @@
         <v>0.01</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E14" t="s">
-        <v>131</v>
+      <c r="E14" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
-        <v>44</v>
+      <c r="G14">
+        <v>0.05</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
         <v>2.8000000000000001E-2</v>
@@ -1638,15 +1625,15 @@
         <v>0.05</v>
       </c>
       <c r="H15" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1661,44 +1648,44 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1">
         <v>0.01</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G17" s="2">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="F18">
         <v>2.9999999999999997E-4</v>
@@ -1707,44 +1694,44 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G19">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
-        <v>87</v>
+      <c r="E20" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1753,73 +1740,73 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>0.04</v>
       </c>
-      <c r="E21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>59</v>
+      <c r="E21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="G21">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H21" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C22">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22" t="s">
-        <v>98</v>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>1E-4</v>
       </c>
       <c r="G22">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -1834,21 +1821,21 @@
         <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
-        <v>87</v>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1857,38 +1844,38 @@
         <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="E26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2">
         <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C27">
         <v>16</v>
@@ -1897,21 +1884,21 @@
         <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -1920,93 +1907,94 @@
         <v>10</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C29">
         <v>13</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G29" s="1">
-        <v>30</v>
-      </c>
+      <c r="E29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="2">
+        <v>100</v>
+      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C30">
         <v>0.2</v>
       </c>
-      <c r="E30" t="s">
-        <v>107</v>
+      <c r="E30" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="G30">
         <v>0.12</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C31">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E31" t="s">
-        <v>75</v>
+      <c r="E31" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0.5</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>0.8</v>
       </c>
-      <c r="E32" t="s">
-        <v>79</v>
+      <c r="E32" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2015,21 +2003,21 @@
         <v>5</v>
       </c>
       <c r="H32" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>1.5</v>
       </c>
-      <c r="E33" t="s">
-        <v>79</v>
+      <c r="E33" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2038,30 +2026,30 @@
         <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>0.95</v>
       </c>
-      <c r="E34" t="s">
-        <v>108</v>
+      <c r="E34" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="F34">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in model structure: removed cancer_prog_constant (age effect cannot be turned off), removed hccr_ic so cancer_prog_coefficient describes the rate to HCC in inactive carriers by definition, progression through eAg-positive compartments is now an exponential GROWTH function
</commit_message>
<xml_diff>
--- a/documentation/priors.xlsx
+++ b/documentation/priors.xlsx
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nora Schmit\Documents\Model development\hbvmodel\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B55CA-A68C-48E6-9570-7140F43ADEF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21344AD-C30F-4A50-AD4F-1BFD2BEA689C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="priors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
   <si>
     <t>Parameter name</t>
   </si>
@@ -79,9 +87,6 @@
     <t>Relative infectiousness of HBeAg-positives compared to HBeAg-negatives for horizontal transmission</t>
   </si>
   <si>
-    <t>alpha needs to be higher than 1 because eAg-positives are more infectious</t>
-  </si>
-  <si>
     <t xml:space="preserve">mtct_prob_e </t>
   </si>
   <si>
@@ -193,12 +198,6 @@
     <t>cancer_prog_coefficient_female</t>
   </si>
   <si>
-    <t>cancer_prog_constant_female</t>
-  </si>
-  <si>
-    <t>Constant term of quadratic shift function for age-specific progression rates to HCC in women. This describes the annual progression rate from Immune tolerant to HCC in women aged cancer_age_threshold+1 (or the average age-independent rate if cancer_prog_coefficient_female = 0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">cancer_age_threshold </t>
   </si>
   <si>
@@ -304,12 +303,6 @@
     <t>Multiplier on progression rate to HCC from Compensated cirrhosis stage compared to from Inactive carrier</t>
   </si>
   <si>
-    <t xml:space="preserve">Normal(0, 0.005)? </t>
-  </si>
-  <si>
-    <t>Depends if we want an increase to be more likely</t>
-  </si>
-  <si>
     <t>0.63 was the minimum reported in the Edmunds study (in Asia). 0.89 is the Edmunds value.</t>
   </si>
   <si>
@@ -395,13 +388,16 @@
   </si>
   <si>
     <t>Normal(6,3) truncated at 1 - center at 6</t>
+  </si>
+  <si>
+    <t>alpha needs to be higher than 1 because eAg-positives are more infectious. See refs in Evernote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,13 +534,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -898,16 +887,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1263,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1320,13 +1308,13 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G2">
         <v>0.7</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1389,21 +1377,21 @@
         <v>10</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
       </c>
       <c r="C6">
         <v>0.6</v>
@@ -1412,27 +1400,27 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7">
         <v>0.05</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1441,21 +1429,21 @@
         <v>0.3</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
       </c>
       <c r="C8">
         <v>0.89</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F8">
         <v>0.65</v>
@@ -1464,21 +1452,21 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
       <c r="C9">
         <v>0.65</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F9">
         <v>0.25</v>
@@ -1487,21 +1475,21 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10">
         <v>0.46</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F10">
         <v>0.1</v>
@@ -1510,21 +1498,21 @@
         <v>0.9</v>
       </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
       </c>
       <c r="C11">
         <v>0.1</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F11">
         <v>0.01</v>
@@ -1533,15 +1521,15 @@
         <v>0.3</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
       </c>
       <c r="C12">
         <v>0.8</v>
@@ -1556,44 +1544,42 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>94</v>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F13" s="2">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
         <v>0.01</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
       </c>
       <c r="C14">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1602,15 +1588,15 @@
         <v>0.05</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
       </c>
       <c r="C15" s="1">
         <v>2.8000000000000001E-2</v>
@@ -1625,15 +1611,15 @@
         <v>0.05</v>
       </c>
       <c r="H15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1648,21 +1634,21 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
       </c>
       <c r="C17" s="1">
         <v>0.01</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F17" s="2">
         <v>0.01</v>
@@ -1671,21 +1657,21 @@
         <v>0.06</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>101</v>
+      <c r="C18" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F18">
         <v>2.9999999999999997E-4</v>
@@ -1693,22 +1679,22 @@
       <c r="G18">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>103</v>
+      <c r="H18" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
       </c>
       <c r="C19" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F19">
         <v>1E-3</v>
@@ -1717,21 +1703,21 @@
         <v>0.05</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1740,41 +1726,41 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
         <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
       </c>
       <c r="C21">
         <v>0.04</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="6">
+        <v>109</v>
+      </c>
+      <c r="F21" s="5">
         <v>0.03</v>
       </c>
       <c r="G21">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22">
-        <v>2.5000000000000001E-4</v>
+        <v>1.25E-4</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>10</v>
@@ -1786,201 +1772,212 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="G23" s="2">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
       <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
         <v>15</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>15</v>
-      </c>
       <c r="H24" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25">
+        <v>119</v>
+      </c>
+      <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G25">
-        <v>15</v>
+      <c r="G25" s="2">
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <v>13</v>
-      </c>
-      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>85</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="G28" s="2">
+        <v>100</v>
+      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C29">
-        <v>13</v>
+        <v>0.2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="2">
-        <v>100</v>
-      </c>
-      <c r="H29" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F29">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="G29">
+        <v>0.12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
       <c r="C30">
-        <v>0.2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F30">
-        <v>7.7000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0.12</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
       <c r="C31">
-        <v>5.0000000000000001E-3</v>
+        <v>0.8</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>6.6000000000000003E-2</v>
+        <v>5</v>
       </c>
       <c r="H31" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1991,10 +1988,10 @@
         <v>72</v>
       </c>
       <c r="C32">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2003,53 +2000,30 @@
         <v>5</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
       <c r="C33">
-        <v>1.5</v>
+        <v>0.95</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="G33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34">
-        <v>0.95</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34">
-        <v>0.7</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed weighting scheme on real calibration data to upweight best quality datapoints in each dataset. Changed priors on age_thresholds to a DISCRETE uniform distribution
</commit_message>
<xml_diff>
--- a/documentation/priors.xlsx
+++ b/documentation/priors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nora Schmit\Documents\Model development\hbvmodel\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21344AD-C30F-4A50-AD4F-1BFD2BEA689C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A9E4F-EB3A-485D-8923-496E7E38709A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
   <si>
     <t>Parameter name</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>alpha needs to be higher than 1 because eAg-positives are more infectious. See refs in Evernote</t>
+  </si>
+  <si>
+    <t>Discrete uniform</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1257,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1625,7 +1628,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -1786,7 +1789,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>

</xml_diff>